<commit_message>
v1.3.1 - pokemon effects - updated data
</commit_message>
<xml_diff>
--- a/src/assets/pokemon_details_list.xlsx
+++ b/src/assets/pokemon_details_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elad\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{494DB7BF-5F66-4C81-86A0-077917C69CFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A18134-7A6B-4618-97DD-33678A822E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="19170" windowHeight="10170" xr2:uid="{7AE0BA4F-9C26-4603-9ABD-3054527CCEB4}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="19140" windowHeight="10170" xr2:uid="{7AE0BA4F-9C26-4603-9ABD-3054527CCEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="341">
   <si>
     <t>pokemon num</t>
   </si>
@@ -1679,33 +1679,6 @@
   </si>
   <si>
     <r>
-      <t>Acid 2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DiceDown(6)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Thunderbolt </t>
     </r>
     <r>
@@ -2112,6 +2085,2331 @@
         <scheme val="minor"/>
       </rPr>
       <t>Diceup(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Acid 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diceup(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Petal Dance 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>???(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Spore </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zzz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sleep Powder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zzz(3)</t>
+    </r>
+  </si>
+  <si>
+    <t>Leech Life 3</t>
+  </si>
+  <si>
+    <t>Earthquake 3</t>
+  </si>
+  <si>
+    <r>
+      <t>Pay Day </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Item(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Slash </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bite 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fury Swipes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fury Swipes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Disable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Low Kick </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Seismic Toss </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1/2LVL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hypnosis </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zzz(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Double slap </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Psychic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reflect </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown2</t>
+    </r>
+  </si>
+  <si>
+    <t>Karate Chop 2</t>
+  </si>
+  <si>
+    <t>Low Kick 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Submission </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Barrier </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Defense Curl </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Self-Destruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO</t>
+    </r>
+  </si>
+  <si>
+    <t>Rock Throw 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Explosion </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stomp </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Take Down </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Swords Dance </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fury Attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fury Attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tri Attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aurora Beam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Headbutt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(5)</t>
+    </r>
+  </si>
+  <si>
+    <t>Take Down 2 KO(6)</t>
+  </si>
+  <si>
+    <r>
+      <t>Ice Beam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frz(6)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pound 1</t>
+  </si>
+  <si>
+    <r>
+      <t>Poison Gas </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psn(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sludge </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psn(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Acid Armor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clamp </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aurora Beam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Confuse Ray </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>???</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dream Eater </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hypnosis </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zzz(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Night Shade </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1/2LVL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bind </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vice Grip </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Guillotine </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO(5)</t>
+    </r>
+  </si>
+  <si>
+    <t>Crabhammer 3</t>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Barrage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bone Club </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bonemerang </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Double Kick </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mega Kick </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mega Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Counter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Slam 3</t>
+  </si>
+  <si>
+    <r>
+      <t>Screech </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Smog </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psn(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Smog </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psn(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Horn Attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Horn Drill </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bind </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dizzy Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>???(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp(Dmg)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Smokescreen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Waterfall </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Double Team </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lovely Kiss </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zzz(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ice Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frz(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Thunder Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Par(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Screech </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fire Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Brn(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vice Grip </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceUp(Dmg)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dragon Rage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IgnoreType</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transform </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bite </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Thunder Wave </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Par(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Thunder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Par(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spike Cannon </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dice+(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hyper Beam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recharge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Double-Edge </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KO(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Body Slam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Par(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Blizzard </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frz(6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Drill Peck </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sky Attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recharge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF9900FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dragon Rage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IgnoreType</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hyper Beam </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recharge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mega Punch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Psychic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceDown(6)</t>
     </r>
   </si>
 </sst>
@@ -2119,7 +4417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2247,6 +4545,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -2364,7 +4683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2468,12 +4787,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2593,6 +4921,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2912,9 +5246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AE034A-BEE3-45F6-9F03-F8448B5D6BAA}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2922,9 +5256,9 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3473,7 +5807,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>11</v>
@@ -3519,13 +5853,13 @@
         <v>41</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>31</v>
@@ -3565,7 +5899,7 @@
         <v>44</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>31</v>
@@ -3634,13 +5968,13 @@
         <v>11</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>74</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>31</v>
@@ -3703,13 +6037,13 @@
         <v>11</v>
       </c>
       <c r="D35" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="38" t="s">
         <v>240</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>241</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>31</v>
@@ -3749,13 +6083,13 @@
         <v>31</v>
       </c>
       <c r="D37" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="37" t="s">
         <v>242</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="37" t="s">
-        <v>243</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>31</v>
@@ -3801,7 +6135,7 @@
         <v>15</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>15</v>
@@ -3841,13 +6175,13 @@
         <v>31</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>31</v>
@@ -3870,7 +6204,7 @@
         <v>24</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>31</v>
@@ -3887,7 +6221,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>31</v>
@@ -3939,13 +6273,13 @@
         <v>10</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36">
         <v>45</v>
       </c>
@@ -3953,6 +6287,18 @@
         <v>62</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>250</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="G46" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3979,7 +6325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="36">
         <v>47</v>
       </c>
@@ -3988,6 +6334,18 @@
       </c>
       <c r="C48" s="13" t="s">
         <v>24</v>
+      </c>
+      <c r="D48" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4000,6 +6358,18 @@
       <c r="C49" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="D49" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="36">
@@ -4011,6 +6381,18 @@
       <c r="C50" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="D50" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="36">
@@ -4035,7 +6417,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="36">
         <v>51</v>
       </c>
@@ -4045,8 +6427,20 @@
       <c r="C52" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D52" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="36">
         <v>52</v>
       </c>
@@ -4054,6 +6448,18 @@
         <v>69</v>
       </c>
       <c r="C53" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="G53" s="14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4067,8 +6473,20 @@
       <c r="C54" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" t="s">
+        <v>257</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="36">
         <v>54</v>
       </c>
@@ -4077,6 +6495,18 @@
       </c>
       <c r="C55" s="11" t="s">
         <v>20</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4089,8 +6519,20 @@
       <c r="C56" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="36">
         <v>56</v>
       </c>
@@ -4100,8 +6542,20 @@
       <c r="C57" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D57" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="36">
         <v>57</v>
       </c>
@@ -4111,8 +6565,20 @@
       <c r="C58" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D58" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="36">
         <v>58</v>
       </c>
@@ -4122,8 +6588,20 @@
       <c r="C59" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D59" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="36">
         <v>59</v>
       </c>
@@ -4133,8 +6611,20 @@
       <c r="C60" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D60" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="36">
         <v>60</v>
       </c>
@@ -4144,8 +6634,20 @@
       <c r="C61" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D61" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="36">
         <v>61</v>
       </c>
@@ -4153,6 +6655,18 @@
         <v>79</v>
       </c>
       <c r="C62" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="G62" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4166,6 +6680,18 @@
       <c r="C63" s="25" t="s">
         <v>20</v>
       </c>
+      <c r="D63" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="36">
@@ -4184,7 +6710,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="36">
         <v>64</v>
       </c>
@@ -4194,8 +6720,20 @@
       <c r="C65" s="26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D65" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F65" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="36">
         <v>65</v>
       </c>
@@ -4203,6 +6741,18 @@
         <v>84</v>
       </c>
       <c r="C66" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F66" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="G66" s="26" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4216,6 +6766,12 @@
       <c r="C67" s="23" t="s">
         <v>74</v>
       </c>
+      <c r="D67" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="36">
@@ -4227,8 +6783,20 @@
       <c r="C68" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D68" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="36">
         <v>68</v>
       </c>
@@ -4236,6 +6804,18 @@
         <v>87</v>
       </c>
       <c r="C69" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="G69" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4262,7 +6842,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="36">
         <v>70</v>
       </c>
@@ -4272,8 +6852,20 @@
       <c r="C71" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D71" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="36">
         <v>71</v>
       </c>
@@ -4282,6 +6874,18 @@
       </c>
       <c r="C72" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4307,7 +6911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="36">
         <v>73</v>
       </c>
@@ -4316,6 +6920,18 @@
       </c>
       <c r="C74" s="25" t="s">
         <v>20</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E74" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="G74" s="26" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4328,8 +6944,20 @@
       <c r="C75" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D75" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F75" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="36">
         <v>75</v>
       </c>
@@ -4337,6 +6965,18 @@
         <v>95</v>
       </c>
       <c r="C76" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="G76" s="27" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4350,6 +6990,18 @@
       <c r="C77" s="27" t="s">
         <v>94</v>
       </c>
+      <c r="D77" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F77" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="G77" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="36">
@@ -4361,6 +7013,18 @@
       <c r="C78" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="D78" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F78" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="79" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="36">
@@ -4372,8 +7036,20 @@
       <c r="C79" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D79" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="36">
         <v>79</v>
       </c>
@@ -4383,8 +7059,20 @@
       <c r="C80" s="28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D80" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="36">
         <v>80</v>
       </c>
@@ -4394,8 +7082,20 @@
       <c r="C81" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D81" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F81" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="36">
         <v>81</v>
       </c>
@@ -4405,8 +7105,20 @@
       <c r="C82" s="30" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D82" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F82" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="36">
         <v>82</v>
       </c>
@@ -4416,8 +7128,20 @@
       <c r="C83" s="30" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D83" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F83" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="36">
         <v>83</v>
       </c>
@@ -4427,8 +7151,20 @@
       <c r="C84" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D84" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F84" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="36">
         <v>84</v>
       </c>
@@ -4438,8 +7174,20 @@
       <c r="C85" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D85" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F85" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="36">
         <v>85</v>
       </c>
@@ -4449,8 +7197,20 @@
       <c r="C86" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D86" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F86" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="36">
         <v>86</v>
       </c>
@@ -4460,8 +7220,20 @@
       <c r="C87" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D87" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="E87" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F87" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="36">
         <v>87</v>
       </c>
@@ -4471,8 +7243,20 @@
       <c r="C88" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D88" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F88" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="G88" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="36">
         <v>88</v>
       </c>
@@ -4482,8 +7266,20 @@
       <c r="C89" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D89" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="E89" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="G89" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="36">
         <v>89</v>
       </c>
@@ -4493,8 +7289,20 @@
       <c r="C90" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D90" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="E90" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="36">
         <v>90</v>
       </c>
@@ -4504,8 +7312,20 @@
       <c r="C91" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D91" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="36">
         <v>91</v>
       </c>
@@ -4515,8 +7335,20 @@
       <c r="C92" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D92" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="E92" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="G92" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="36">
         <v>92</v>
       </c>
@@ -4533,7 +7365,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="36">
         <v>93</v>
       </c>
@@ -4543,8 +7375,20 @@
       <c r="C94" s="32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D94" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="G94" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="36">
         <v>94</v>
       </c>
@@ -4554,8 +7398,20 @@
       <c r="C95" s="32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D95" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="E95" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F95" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="G95" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="36">
         <v>95</v>
       </c>
@@ -4564,6 +7420,18 @@
       </c>
       <c r="C96" s="27" t="s">
         <v>94</v>
+      </c>
+      <c r="D96" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F96" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G96" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4589,7 +7457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="36">
         <v>97</v>
       </c>
@@ -4597,6 +7465,18 @@
         <v>119</v>
       </c>
       <c r="C98" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D98" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F98" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="G98" s="26" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4610,8 +7490,20 @@
       <c r="C99" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D99" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="E99" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F99" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="36">
         <v>99</v>
       </c>
@@ -4621,8 +7513,20 @@
       <c r="C100" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D100" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F100" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="36">
         <v>100</v>
       </c>
@@ -4631,6 +7535,18 @@
       </c>
       <c r="C101" s="17" t="s">
         <v>41</v>
+      </c>
+      <c r="D101" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="E101" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F101" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="G101" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4643,8 +7559,20 @@
       <c r="C102" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D102" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="E102" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F102" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G102" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="36">
         <v>102</v>
       </c>
@@ -4653,6 +7581,18 @@
       </c>
       <c r="C103" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="E103" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F103" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="G103" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4665,6 +7605,18 @@
       <c r="C104" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="D104" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="G104" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="105" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="36">
@@ -4676,8 +7628,20 @@
       <c r="C105" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D105" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F105" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="G105" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="36">
         <v>105</v>
       </c>
@@ -4687,8 +7651,20 @@
       <c r="C106" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D106" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="E106" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F106" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G106" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="36">
         <v>106</v>
       </c>
@@ -4698,8 +7674,20 @@
       <c r="C107" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D107" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F107" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="G107" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="36">
         <v>107</v>
       </c>
@@ -4709,8 +7697,20 @@
       <c r="C108" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D108" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="E108" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F108" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="G108" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="36">
         <v>108</v>
       </c>
@@ -4720,8 +7720,20 @@
       <c r="C109" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D109" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="E109" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F109" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="G109" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="36">
         <v>109</v>
       </c>
@@ -4731,8 +7743,20 @@
       <c r="C110" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D110" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G110" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="36">
         <v>110</v>
       </c>
@@ -4742,8 +7766,20 @@
       <c r="C111" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D111" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="E111" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F111" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="G111" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="36">
         <v>111</v>
       </c>
@@ -4752,6 +7788,18 @@
       </c>
       <c r="C112" s="19" t="s">
         <v>44</v>
+      </c>
+      <c r="D112" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F112" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="G112" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4764,8 +7812,20 @@
       <c r="C113" s="19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D113" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F113" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="G113" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="36">
         <v>113</v>
       </c>
@@ -4775,8 +7835,20 @@
       <c r="C114" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D114" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F114" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="G114" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="36">
         <v>114</v>
       </c>
@@ -4786,8 +7858,20 @@
       <c r="C115" s="33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D115" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="G115" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="36">
         <v>115</v>
       </c>
@@ -4795,6 +7879,18 @@
         <v>137</v>
       </c>
       <c r="C116" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D116" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F116" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="G116" s="15" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4808,6 +7904,18 @@
       <c r="C117" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="D117" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F117" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="G117" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="118" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="36">
@@ -4819,6 +7927,18 @@
       <c r="C118" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="D118" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="E118" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F118" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="119" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="36">
@@ -4843,7 +7963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="36">
         <v>119</v>
       </c>
@@ -4851,6 +7971,18 @@
         <v>141</v>
       </c>
       <c r="C120" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D120" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="E120" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F120" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="G120" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4864,6 +7996,18 @@
       <c r="C121" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="D121" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F121" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G121" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="122" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="36">
@@ -4875,8 +8019,20 @@
       <c r="C122" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D122" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F122" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G122" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="36">
         <v>122</v>
       </c>
@@ -4886,8 +8042,20 @@
       <c r="C123" s="29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D123" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E123" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F123" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="G123" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="36">
         <v>123</v>
       </c>
@@ -4897,8 +8065,20 @@
       <c r="C124" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D124" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="E124" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F124" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="G124" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="36">
         <v>124</v>
       </c>
@@ -4906,6 +8086,18 @@
         <v>146</v>
       </c>
       <c r="C125" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D125" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="E125" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F125" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="G125" s="31" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4919,8 +8111,20 @@
       <c r="C126" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D126" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="E126" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F126" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="G126" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="36">
         <v>126</v>
       </c>
@@ -4930,8 +8134,20 @@
       <c r="C127" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D127" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F127" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="36">
         <v>127</v>
       </c>
@@ -4940,6 +8156,18 @@
       </c>
       <c r="C128" s="12" t="s">
         <v>24</v>
+      </c>
+      <c r="D128" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="E128" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F128" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="G128" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4952,6 +8180,18 @@
       <c r="C129" s="15" t="s">
         <v>31</v>
       </c>
+      <c r="D129" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="E129" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F129" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="G129" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="130" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="36">
@@ -4970,7 +8210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="36">
         <v>130</v>
       </c>
@@ -4980,8 +8220,20 @@
       <c r="C131" s="25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D131" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="E131" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F131" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G131" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="36">
         <v>131</v>
       </c>
@@ -4990,6 +8242,18 @@
       </c>
       <c r="C132" s="25" t="s">
         <v>20</v>
+      </c>
+      <c r="D132" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="E132" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F132" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="G132" s="31" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -5002,8 +8266,14 @@
       <c r="C133" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D133" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="E133" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="36">
         <v>133</v>
       </c>
@@ -5013,8 +8283,20 @@
       <c r="C134" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D134" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="E134" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F134" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="G134" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="36">
         <v>134</v>
       </c>
@@ -5022,6 +8304,18 @@
         <v>156</v>
       </c>
       <c r="C135" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D135" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="E135" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F135" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G135" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5035,8 +8329,20 @@
       <c r="C136" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D136" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="E136" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F136" s="38" t="s">
+        <v>329</v>
+      </c>
+      <c r="G136" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A137" s="36">
         <v>136</v>
       </c>
@@ -5044,6 +8350,18 @@
         <v>158</v>
       </c>
       <c r="C137" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F137" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="G137" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5080,6 +8398,18 @@
       <c r="C139" s="27" t="s">
         <v>94</v>
       </c>
+      <c r="D139" s="39" t="s">
+        <v>330</v>
+      </c>
+      <c r="E139" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F139" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="G139" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="140" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="36">
@@ -5091,6 +8421,18 @@
       <c r="C140" s="27" t="s">
         <v>94</v>
       </c>
+      <c r="D140" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E140" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F140" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="G140" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="141" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="36">
@@ -5102,8 +8444,20 @@
       <c r="C141" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D141" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E141" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F141" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G141" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="36">
         <v>141</v>
       </c>
@@ -5113,8 +8467,20 @@
       <c r="C142" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D142" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E142" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F142" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="G142" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="36">
         <v>142</v>
       </c>
@@ -5124,8 +8490,20 @@
       <c r="C143" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D143" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="E143" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F143" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="G143" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="36">
         <v>143</v>
       </c>
@@ -5135,8 +8513,20 @@
       <c r="C144" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D144" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="E144" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F144" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="G144" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="36">
         <v>144</v>
       </c>
@@ -5146,8 +8536,20 @@
       <c r="C145" s="31" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D145" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="E145" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F145" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G145" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="36">
         <v>145</v>
       </c>
@@ -5157,8 +8559,20 @@
       <c r="C146" s="30" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D146" s="38" t="s">
+        <v>329</v>
+      </c>
+      <c r="E146" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F146" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="36">
         <v>146</v>
       </c>
@@ -5166,6 +8580,18 @@
         <v>168</v>
       </c>
       <c r="C147" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="E147" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F147" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="G147" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5202,8 +8628,20 @@
       <c r="C149" s="34" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D149" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="E149" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F149" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G149" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="36">
         <v>149</v>
       </c>
@@ -5212,6 +8650,18 @@
       </c>
       <c r="C150" s="35" t="s">
         <v>170</v>
+      </c>
+      <c r="D150" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="E150" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F150" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="G150" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -5224,6 +8674,18 @@
       <c r="C151" s="26" t="s">
         <v>82</v>
       </c>
+      <c r="D151" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="E151" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F151" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G151" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="152" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="36">
@@ -5233,6 +8695,18 @@
         <v>174</v>
       </c>
       <c r="C152" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D152" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="E152" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F152" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="G152" s="26" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5272,6 +8746,7 @@
     <hyperlink ref="C37" r:id="rId32" location="cite_note-NormaltoFairy-17" display="cite_note-NormaltoFairy-17" xr:uid="{34A3B7D1-004F-43BB-BCEE-CDECC419528E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
v1.3.2 - pokemon effects - improved css + evolutions + bg image
</commit_message>
<xml_diff>
--- a/src/assets/pokemon_details_list.xlsx
+++ b/src/assets/pokemon_details_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elad\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A18134-7A6B-4618-97DD-33678A822E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742002BA-3184-4C42-95C2-B1308C9980C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="19140" windowHeight="10170" xr2:uid="{7AE0BA4F-9C26-4603-9ABD-3054527CCEB4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="342">
   <si>
     <t>pokemon num</t>
   </si>
@@ -4411,6 +4411,9 @@
       </rPr>
       <t>DiceDown(6)</t>
     </r>
+  </si>
+  <si>
+    <t>evolve</t>
   </si>
 </sst>
 </file>
@@ -5244,11 +5247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AE034A-BEE3-45F6-9F03-F8448B5D6BAA}">
-  <dimension ref="A1:G152"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5262,7 +5265,7 @@
     <col min="7" max="7" width="9.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5284,8 +5287,11 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -5307,8 +5313,11 @@
       <c r="G2" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36">
         <v>2</v>
       </c>
@@ -5330,8 +5339,11 @@
       <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36">
         <v>3</v>
       </c>
@@ -5354,7 +5366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36">
         <v>4</v>
       </c>
@@ -5376,8 +5388,11 @@
       <c r="G5" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H5" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="36">
         <v>5</v>
       </c>
@@ -5399,8 +5414,11 @@
       <c r="G6" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36">
         <v>6</v>
       </c>
@@ -5423,7 +5441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36">
         <v>7</v>
       </c>
@@ -5445,8 +5463,11 @@
       <c r="G8" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36">
         <v>8</v>
       </c>
@@ -5468,8 +5489,11 @@
       <c r="G9" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="36">
         <v>9</v>
       </c>
@@ -5492,7 +5516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36">
         <v>10</v>
       </c>
@@ -5508,8 +5532,11 @@
       <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36">
         <v>11</v>
       </c>
@@ -5531,8 +5558,11 @@
       <c r="G12" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36">
         <v>12</v>
       </c>
@@ -5555,7 +5585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36">
         <v>13</v>
       </c>
@@ -5571,8 +5601,11 @@
       <c r="E14" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36">
         <v>14</v>
       </c>
@@ -5594,8 +5627,11 @@
       <c r="G15" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="36">
         <v>15</v>
       </c>
@@ -5618,7 +5654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="36">
         <v>16</v>
       </c>
@@ -5634,8 +5670,11 @@
       <c r="E17" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="36">
         <v>17</v>
       </c>
@@ -5657,8 +5696,11 @@
       <c r="G18" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="36">
         <v>18</v>
       </c>
@@ -5681,7 +5723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="36">
         <v>19</v>
       </c>
@@ -5703,8 +5745,11 @@
       <c r="G20" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="36">
         <v>20</v>
       </c>
@@ -5727,7 +5772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="36">
         <v>21</v>
       </c>
@@ -5749,8 +5794,11 @@
       <c r="G22" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="36">
         <v>22</v>
       </c>
@@ -5773,7 +5821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="36">
         <v>23</v>
       </c>
@@ -5795,8 +5843,11 @@
       <c r="G24" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="36">
         <v>24</v>
       </c>
@@ -5819,7 +5870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="36">
         <v>25</v>
       </c>
@@ -5841,8 +5892,11 @@
       <c r="G26" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="36">
         <v>26</v>
       </c>
@@ -5865,7 +5919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="36">
         <v>27</v>
       </c>
@@ -5887,8 +5941,11 @@
       <c r="G28" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="36">
         <v>28</v>
       </c>
@@ -5911,7 +5968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="36">
         <v>29</v>
       </c>
@@ -5933,8 +5990,11 @@
       <c r="G30" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="36">
         <v>30</v>
       </c>
@@ -5956,8 +6016,11 @@
       <c r="G31" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="36">
         <v>31</v>
       </c>
@@ -5980,7 +6043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="36">
         <v>32</v>
       </c>
@@ -6002,8 +6065,11 @@
       <c r="G33" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H33" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="36">
         <v>33</v>
       </c>
@@ -6025,8 +6091,11 @@
       <c r="G34" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="36">
         <v>34</v>
       </c>
@@ -6049,7 +6118,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="36">
         <v>35</v>
       </c>
@@ -6071,8 +6140,11 @@
       <c r="G36" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="36">
         <v>36</v>
       </c>
@@ -6095,7 +6167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="36">
         <v>37</v>
       </c>
@@ -6117,8 +6189,11 @@
       <c r="G38" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H38" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="36">
         <v>38</v>
       </c>
@@ -6141,7 +6216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="36">
         <v>39</v>
       </c>
@@ -6163,8 +6238,11 @@
       <c r="G40" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="36">
         <v>40</v>
       </c>
@@ -6187,7 +6265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="36">
         <v>41</v>
       </c>
@@ -6209,8 +6287,11 @@
       <c r="G42" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H42" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="36">
         <v>42</v>
       </c>
@@ -6233,7 +6314,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="36">
         <v>43</v>
       </c>
@@ -6255,8 +6336,11 @@
       <c r="G44" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H44" s="36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="36">
         <v>44</v>
       </c>
@@ -6278,8 +6362,11 @@
       <c r="G45" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H45" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36">
         <v>45</v>
       </c>
@@ -6302,7 +6389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="36">
         <v>46</v>
       </c>
@@ -6324,8 +6411,11 @@
       <c r="G47" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H47" s="36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="36">
         <v>47</v>
       </c>
@@ -6348,7 +6438,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="36">
         <v>48</v>
       </c>
@@ -6370,8 +6460,11 @@
       <c r="G49" s="26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H49" s="36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="36">
         <v>49</v>
       </c>
@@ -6394,7 +6487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="36">
         <v>50</v>
       </c>
@@ -6416,8 +6509,11 @@
       <c r="G51" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H51" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="36">
         <v>51</v>
       </c>
@@ -6440,7 +6536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="36">
         <v>52</v>
       </c>
@@ -6462,8 +6558,11 @@
       <c r="G53" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H53" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="36">
         <v>53</v>
       </c>
@@ -6486,7 +6585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="36">
         <v>54</v>
       </c>
@@ -6508,8 +6607,11 @@
       <c r="G55" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H55" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="36">
         <v>55</v>
       </c>
@@ -6532,7 +6634,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="36">
         <v>56</v>
       </c>
@@ -6554,8 +6656,11 @@
       <c r="G57" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H57" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="36">
         <v>57</v>
       </c>
@@ -6578,7 +6683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="36">
         <v>58</v>
       </c>
@@ -6600,8 +6705,11 @@
       <c r="G59" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H59" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="36">
         <v>59</v>
       </c>
@@ -6624,7 +6732,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="36">
         <v>60</v>
       </c>
@@ -6646,8 +6754,11 @@
       <c r="G61" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H61" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="36">
         <v>61</v>
       </c>
@@ -6669,8 +6780,11 @@
       <c r="G62" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H62" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="36">
         <v>62</v>
       </c>
@@ -6693,7 +6807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="36">
         <v>63</v>
       </c>
@@ -6709,8 +6823,11 @@
       <c r="E64" s="26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H64" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="36">
         <v>64</v>
       </c>
@@ -6732,8 +6849,11 @@
       <c r="G65" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H65" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="36">
         <v>65</v>
       </c>
@@ -6756,7 +6876,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="36">
         <v>66</v>
       </c>
@@ -6772,8 +6892,11 @@
       <c r="E67" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H67" s="36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="36">
         <v>67</v>
       </c>
@@ -6795,8 +6918,11 @@
       <c r="G68" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H68" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="36">
         <v>68</v>
       </c>
@@ -6819,7 +6945,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="36">
         <v>69</v>
       </c>
@@ -6841,8 +6967,11 @@
       <c r="G70" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="36">
         <v>70</v>
       </c>
@@ -6864,8 +6993,11 @@
       <c r="G71" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H71" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="36">
         <v>71</v>
       </c>
@@ -6888,7 +7020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="36">
         <v>72</v>
       </c>
@@ -6910,8 +7042,11 @@
       <c r="G73" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H73" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="36">
         <v>73</v>
       </c>
@@ -6934,7 +7069,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="36">
         <v>74</v>
       </c>
@@ -6956,8 +7091,11 @@
       <c r="G75" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H75" s="36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="36">
         <v>75</v>
       </c>
@@ -6979,8 +7117,11 @@
       <c r="G76" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H76" s="36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="36">
         <v>76</v>
       </c>
@@ -7003,7 +7144,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="36">
         <v>77</v>
       </c>
@@ -7025,8 +7166,11 @@
       <c r="G78" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H78" s="36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="36">
         <v>78</v>
       </c>
@@ -7049,7 +7193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="36">
         <v>79</v>
       </c>
@@ -7071,8 +7215,11 @@
       <c r="G80" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H80" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="36">
         <v>80</v>
       </c>
@@ -7095,7 +7242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="36">
         <v>81</v>
       </c>
@@ -7117,8 +7264,11 @@
       <c r="G82" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H82" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="36">
         <v>82</v>
       </c>
@@ -7141,7 +7291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="36">
         <v>83</v>
       </c>
@@ -7163,8 +7313,11 @@
       <c r="G84" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H84" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="36">
         <v>84</v>
       </c>
@@ -7187,7 +7340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="36">
         <v>85</v>
       </c>
@@ -7210,7 +7363,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="36">
         <v>86</v>
       </c>
@@ -7232,8 +7385,11 @@
       <c r="G87" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H87" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="36">
         <v>87</v>
       </c>
@@ -7256,7 +7412,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="36">
         <v>88</v>
       </c>
@@ -7278,8 +7434,11 @@
       <c r="G89" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H89" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="36">
         <v>89</v>
       </c>
@@ -7302,7 +7461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="36">
         <v>90</v>
       </c>
@@ -7324,8 +7483,11 @@
       <c r="G91" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H91" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="36">
         <v>91</v>
       </c>
@@ -7348,7 +7510,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="36">
         <v>92</v>
       </c>
@@ -7364,8 +7526,11 @@
       <c r="E93" s="32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H93" s="36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="36">
         <v>93</v>
       </c>
@@ -7387,8 +7552,11 @@
       <c r="G94" s="26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H94" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="36">
         <v>94</v>
       </c>
@@ -7411,7 +7579,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="36">
         <v>95</v>
       </c>
@@ -7433,8 +7601,9 @@
       <c r="G96" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H96" s="36"/>
+    </row>
+    <row r="97" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="36">
         <v>96</v>
       </c>
@@ -7456,8 +7625,11 @@
       <c r="G97" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H97" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="36">
         <v>97</v>
       </c>
@@ -7480,7 +7652,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="36">
         <v>98</v>
       </c>
@@ -7502,8 +7674,11 @@
       <c r="G99" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H99" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="36">
         <v>99</v>
       </c>
@@ -7526,7 +7701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="36">
         <v>100</v>
       </c>
@@ -7548,8 +7723,11 @@
       <c r="G101" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H101" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="36">
         <v>101</v>
       </c>
@@ -7572,7 +7750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="36">
         <v>102</v>
       </c>
@@ -7594,8 +7772,11 @@
       <c r="G103" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H103" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="36">
         <v>103</v>
       </c>
@@ -7618,7 +7799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="36">
         <v>104</v>
       </c>
@@ -7640,8 +7821,11 @@
       <c r="G105" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H105" s="36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="36">
         <v>105</v>
       </c>
@@ -7664,7 +7848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="36">
         <v>106</v>
       </c>
@@ -7687,7 +7871,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="36">
         <v>107</v>
       </c>
@@ -7710,7 +7894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="36">
         <v>108</v>
       </c>
@@ -7733,7 +7917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="36">
         <v>109</v>
       </c>
@@ -7755,8 +7939,11 @@
       <c r="G110" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H110" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="36">
         <v>110</v>
       </c>
@@ -7779,7 +7966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="36">
         <v>111</v>
       </c>
@@ -7801,8 +7988,11 @@
       <c r="G112" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H112" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="36">
         <v>112</v>
       </c>
@@ -7825,7 +8015,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="36">
         <v>113</v>
       </c>
@@ -7848,7 +8038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="36">
         <v>114</v>
       </c>
@@ -7871,7 +8061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="36">
         <v>115</v>
       </c>
@@ -7894,7 +8084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="36">
         <v>116</v>
       </c>
@@ -7916,8 +8106,11 @@
       <c r="G117" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H117" s="36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="36">
         <v>117</v>
       </c>
@@ -7940,7 +8133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="36">
         <v>118</v>
       </c>
@@ -7962,8 +8155,11 @@
       <c r="G119" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H119" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="36">
         <v>119</v>
       </c>
@@ -7986,7 +8182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="36">
         <v>120</v>
       </c>
@@ -8008,8 +8204,11 @@
       <c r="G121" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H121" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="36">
         <v>121</v>
       </c>
@@ -8032,7 +8231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="36">
         <v>122</v>
       </c>
@@ -8055,7 +8254,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="36">
         <v>123</v>
       </c>
@@ -8078,7 +8277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="36">
         <v>124</v>
       </c>
@@ -8101,7 +8300,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="36">
         <v>125</v>
       </c>
@@ -8124,7 +8323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="36">
         <v>126</v>
       </c>
@@ -8147,7 +8346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="36">
         <v>127</v>
       </c>
@@ -8170,7 +8369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="36">
         <v>128</v>
       </c>
@@ -8193,7 +8392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="36">
         <v>129</v>
       </c>
@@ -8209,8 +8408,11 @@
       <c r="E130" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H130" s="36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="36">
         <v>130</v>
       </c>
@@ -8233,7 +8435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="36">
         <v>131</v>
       </c>
@@ -8256,7 +8458,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="36">
         <v>132</v>
       </c>
@@ -8273,7 +8475,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="36">
         <v>133</v>
       </c>
@@ -8295,8 +8497,11 @@
       <c r="G134" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H134" s="36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="36">
         <v>134</v>
       </c>
@@ -8318,8 +8523,11 @@
       <c r="G135" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H135" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="36">
         <v>135</v>
       </c>
@@ -8341,8 +8549,11 @@
       <c r="G136" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H136" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A137" s="36">
         <v>136</v>
       </c>
@@ -8365,7 +8576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="36">
         <v>137</v>
       </c>
@@ -8388,7 +8599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="36">
         <v>138</v>
       </c>
@@ -8410,8 +8621,11 @@
       <c r="G139" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H139" s="36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="36">
         <v>139</v>
       </c>
@@ -8434,7 +8648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="36">
         <v>140</v>
       </c>
@@ -8456,8 +8670,11 @@
       <c r="G141" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H141" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="36">
         <v>141</v>
       </c>
@@ -8480,7 +8697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="36">
         <v>142</v>
       </c>
@@ -8503,7 +8720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="36">
         <v>143</v>
       </c>
@@ -8526,7 +8743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="36">
         <v>144</v>
       </c>
@@ -8549,7 +8766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="36">
         <v>145</v>
       </c>
@@ -8572,7 +8789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="36">
         <v>146</v>
       </c>
@@ -8595,7 +8812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="36">
         <v>147</v>
       </c>
@@ -8617,8 +8834,11 @@
       <c r="G148" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H148" s="36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="36">
         <v>148</v>
       </c>
@@ -8640,8 +8860,11 @@
       <c r="G149" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H149" s="36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="36">
         <v>149</v>
       </c>
@@ -8664,7 +8887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="36">
         <v>150</v>
       </c>
@@ -8687,7 +8910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="36">
         <v>151</v>
       </c>
@@ -8744,9 +8967,19 @@
     <hyperlink ref="B152" r:id="rId30" tooltip="Mew (Pokémon)" display="https://en.wikipedia.org/wiki/Mew_(Pok%C3%A9mon)" xr:uid="{2EDA2396-B49B-4D01-A6FF-A657CA28D1AC}"/>
     <hyperlink ref="C36" r:id="rId31" location="cite_note-NormaltoFairy-17" display="cite_note-NormaltoFairy-17" xr:uid="{A1ED406F-759F-4D80-85A6-77794ECD8C3B}"/>
     <hyperlink ref="C37" r:id="rId32" location="cite_note-NormaltoFairy-17" display="cite_note-NormaltoFairy-17" xr:uid="{34A3B7D1-004F-43BB-BCEE-CDECC419528E}"/>
+    <hyperlink ref="H3" r:id="rId33" tooltip="Venusaur" display="https://en.wikipedia.org/wiki/Venusaur" xr:uid="{691BC9AE-E1DE-4F9C-9382-2281C06A84BC}"/>
+    <hyperlink ref="H6" r:id="rId34" tooltip="Charizard" display="https://en.wikipedia.org/wiki/Charizard" xr:uid="{4B3A3584-F382-4D6C-8939-8D257F4B5C12}"/>
+    <hyperlink ref="H9" r:id="rId35" tooltip="Blastoise" display="https://en.wikipedia.org/wiki/Blastoise" xr:uid="{691C2B0A-C652-46D3-90F1-EF38FDE9D497}"/>
+    <hyperlink ref="H38" r:id="rId36" tooltip="Vulpix and Ninetales" display="https://en.wikipedia.org/wiki/Vulpix_and_Ninetales" xr:uid="{116508D8-8F3D-4AD1-81B1-C0479C736D91}"/>
+    <hyperlink ref="H64" r:id="rId37" tooltip="Abra, Kadabra, and Alakazam" display="https://en.wikipedia.org/wiki/Abra,_Kadabra,_and_Alakazam" xr:uid="{6A37282D-AAFB-4A99-9D30-E32CE4492BA6}"/>
+    <hyperlink ref="H65" r:id="rId38" tooltip="Abra, Kadabra, and Alakazam" display="https://en.wikipedia.org/wiki/Abra,_Kadabra,_and_Alakazam" xr:uid="{241AF3E7-5E54-433D-8F6D-C891C37B7C03}"/>
+    <hyperlink ref="H93" r:id="rId39" tooltip="Haunter" display="https://en.wikipedia.org/wiki/Haunter" xr:uid="{3435A796-160E-4B02-8638-B78FD0CF3212}"/>
+    <hyperlink ref="H94" r:id="rId40" tooltip="Gengar" display="https://en.wikipedia.org/wiki/Gengar" xr:uid="{1D597C57-B18C-4F05-A18C-A9B3DAF12894}"/>
+    <hyperlink ref="H110" r:id="rId41" tooltip="Koffing and Weezing" display="https://en.wikipedia.org/wiki/Koffing_and_Weezing" xr:uid="{2AC5B72B-A2B1-4501-8329-F39F5AEC3A76}"/>
+    <hyperlink ref="H130" r:id="rId42" tooltip="Gyarados" display="https://en.wikipedia.org/wiki/Gyarados" xr:uid="{5C751D5D-9165-4619-B619-465C7EECDA90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId43"/>
 </worksheet>
 </file>
 

</xml_diff>